<commit_message>
Agregar archivos de recursos semana 09
</commit_message>
<xml_diff>
--- a/santillana-recursos/semana_07/LGS1_Aprende en casa_GAVI_Semana 7_2021-2022.xlsx
+++ b/santillana-recursos/semana_07/LGS1_Aprende en casa_GAVI_Semana 7_2021-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fceron/Desktop/APRENDE EN CASA/SEMANA 7/DEFINITIVOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos.ciddelapaz/Library/Mobile Documents/com~apple~CloudDocs/Dev/GitHub/gavi/santillana-recursos/semana_07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63BA191-F1C4-084C-9898-8DB63BC36B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE6697D-0A97-D441-B150-CBF07481FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="460" windowWidth="37000" windowHeight="25920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 7" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="121">
   <si>
     <t xml:space="preserve">Páginas de La Guía Santillana </t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Conocimiento del Medio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matemáticas </t>
   </si>
   <si>
     <t>Educación Socioemocional</t>
@@ -500,21 +497,6 @@
   <si>
     <t>Utiliza, con apoyo de un mediador, técnicas para el control de impulsos provocados por
  emociones aflictivas.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">LGS 1: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>116 y 117</t>
-    </r>
   </si>
   <si>
     <r>
@@ -886,6 +868,9 @@
       </rPr>
       <t>37</t>
     </r>
+  </si>
+  <si>
+    <t>Matemáticas +D39:E39</t>
   </si>
 </sst>
 </file>
@@ -1961,6 +1946,108 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1976,37 +2063,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2024,102 +2093,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2435,8 +2420,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="M32" zoomScale="181" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2452,482 +2437,482 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34" customHeight="1">
-      <c r="A1" s="108" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
+      <c r="A1" s="142" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
     </row>
     <row r="2" spans="1:9" ht="32" customHeight="1">
       <c r="A2" s="36"/>
-      <c r="B2" s="124" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
+      <c r="B2" s="152" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
       <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="126" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="128"/>
+      <c r="A3" s="154" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="156"/>
       <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="33" customHeight="1">
       <c r="A4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="E4" s="28" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>10</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:9" ht="63" customHeight="1">
-      <c r="A5" s="112" t="s">
-        <v>33</v>
+      <c r="A5" s="146" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="94" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="95" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" s="93" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="95" t="s">
-        <v>39</v>
       </c>
       <c r="F5" s="96"/>
       <c r="G5" s="97" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H5" s="98"/>
       <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:9" ht="63" customHeight="1">
-      <c r="A6" s="132"/>
+      <c r="A6" s="131"/>
       <c r="B6" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="3"/>
       <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:9" ht="80" customHeight="1">
-      <c r="A7" s="132"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="44"/>
       <c r="H7" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="38"/>
+    </row>
+    <row r="8" spans="1:9" ht="50" customHeight="1">
+      <c r="A8" s="131"/>
+      <c r="B8" s="146" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="159" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="108" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="110" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="114"/>
+      <c r="H8" s="115" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" ht="50" customHeight="1">
+      <c r="A9" s="131"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="1:9" ht="99" customHeight="1">
+      <c r="A10" s="132"/>
+      <c r="B10" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="103" t="s">
         <v>106</v>
-      </c>
-      <c r="I7" s="38"/>
-    </row>
-    <row r="8" spans="1:9" ht="50" customHeight="1">
-      <c r="A8" s="132"/>
-      <c r="B8" s="112" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="133" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="154" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="155" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="156" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="157"/>
-      <c r="H8" s="158" t="s">
-        <v>107</v>
-      </c>
-      <c r="I8" s="38"/>
-    </row>
-    <row r="9" spans="1:9" ht="50" customHeight="1">
-      <c r="A9" s="132"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="134"/>
-      <c r="D9" s="152"/>
-      <c r="E9" s="153"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="38"/>
-    </row>
-    <row r="10" spans="1:9" ht="99" customHeight="1">
-      <c r="A10" s="113"/>
-      <c r="B10" s="90" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="103" t="s">
-        <v>108</v>
       </c>
       <c r="H10" s="47"/>
       <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:9" ht="19" customHeight="1">
-      <c r="A11" s="130"/>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="131"/>
+      <c r="A11" s="157"/>
+      <c r="B11" s="158"/>
+      <c r="C11" s="158"/>
+      <c r="D11" s="158"/>
+      <c r="E11" s="158"/>
+      <c r="F11" s="158"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="158"/>
       <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:9" ht="32">
       <c r="A12" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="D12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="E12" s="28" t="s">
         <v>9</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>10</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="I12" s="38"/>
+    </row>
+    <row r="13" spans="1:9" ht="68" customHeight="1">
+      <c r="A13" s="124" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="1:9" ht="68" customHeight="1">
-      <c r="A13" s="129" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="1:9" ht="96" customHeight="1">
+      <c r="A14" s="124"/>
+      <c r="B14" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="38"/>
-    </row>
-    <row r="14" spans="1:9" ht="96" customHeight="1">
-      <c r="A14" s="129"/>
-      <c r="B14" s="47" t="s">
-        <v>48</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:9" ht="83" customHeight="1">
-      <c r="A15" s="129"/>
+      <c r="A15" s="124"/>
       <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>50</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="68" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:9" ht="102" customHeight="1">
-      <c r="A16" s="129"/>
+      <c r="A16" s="124"/>
       <c r="B16" s="59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16" s="105" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16" s="60"/>
       <c r="H16" s="69"/>
       <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:9" ht="80" customHeight="1">
-      <c r="A17" s="129"/>
+      <c r="A17" s="124"/>
       <c r="B17" s="61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F17" s="106" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="73"/>
       <c r="H17" s="74"/>
       <c r="I17" s="38"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="138"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="138"/>
+      <c r="A18" s="118"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
       <c r="I18" s="38"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="143"/>
-      <c r="B19" s="143"/>
-      <c r="C19" s="143"/>
-      <c r="D19" s="143"/>
-      <c r="E19" s="143"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="143"/>
+      <c r="A19" s="120"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
       <c r="I19" s="38"/>
     </row>
     <row r="20" spans="1:9" ht="32">
       <c r="A20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="D20" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="E20" s="28" t="s">
         <v>9</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>10</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>0</v>
       </c>
       <c r="G20" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="I20" s="38"/>
+    </row>
+    <row r="21" spans="1:9" ht="80" customHeight="1">
+      <c r="A21" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="I20" s="38"/>
-    </row>
-    <row r="21" spans="1:9" ht="80" customHeight="1">
-      <c r="A21" s="129" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="91" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F21" s="58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:9" ht="72" customHeight="1">
-      <c r="A22" s="129"/>
+      <c r="A22" s="124"/>
       <c r="B22" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E22" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" ht="72" customHeight="1">
+      <c r="A23" s="124"/>
+      <c r="B23" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="99" t="s">
         <v>109</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="1:9" ht="72" customHeight="1">
-      <c r="A23" s="129"/>
-      <c r="B23" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="99" t="s">
-        <v>111</v>
       </c>
       <c r="G23" s="32"/>
       <c r="H23" s="75" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I23" s="38"/>
     </row>
     <row r="24" spans="1:9" ht="72" customHeight="1">
-      <c r="A24" s="129"/>
+      <c r="A24" s="124"/>
       <c r="B24" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="66" t="s">
         <v>57</v>
-      </c>
-      <c r="C24" s="78" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="79" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="66" t="s">
-        <v>58</v>
       </c>
       <c r="F24" s="80"/>
       <c r="G24" s="81"/>
@@ -2935,384 +2920,382 @@
       <c r="I24" s="38"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="129"/>
-      <c r="B25" s="132" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="134" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="152" t="s">
+      <c r="A25" s="124"/>
+      <c r="B25" s="131" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="133" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="109" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="153" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="151" t="s">
+      <c r="F25" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="113"/>
+      <c r="H25" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="123"/>
-      <c r="H25" s="110" t="s">
-        <v>29</v>
-      </c>
       <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:9" ht="94" customHeight="1">
-      <c r="A26" s="129"/>
-      <c r="B26" s="113"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="121"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="111"/>
+      <c r="A26" s="124"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="145"/>
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="147"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="147"/>
+      <c r="A27" s="125"/>
+      <c r="B27" s="125"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="125"/>
+      <c r="F27" s="125"/>
+      <c r="G27" s="125"/>
+      <c r="H27" s="125"/>
       <c r="I27" s="38"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="148"/>
-      <c r="B28" s="148"/>
-      <c r="C28" s="148"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="148"/>
-      <c r="F28" s="148"/>
-      <c r="G28" s="148"/>
-      <c r="H28" s="148"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="126"/>
       <c r="I28" s="38"/>
     </row>
     <row r="29" spans="1:9" ht="32">
       <c r="A29" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="C29" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="D29" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="E29" s="28" t="s">
         <v>9</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>10</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>0</v>
       </c>
       <c r="G29" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="I29" s="38"/>
+    </row>
+    <row r="30" spans="1:9" ht="77" customHeight="1">
+      <c r="A30" s="124" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="38"/>
-    </row>
-    <row r="30" spans="1:9" ht="77" customHeight="1">
-      <c r="A30" s="129" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F30" s="107" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I30" s="38"/>
     </row>
     <row r="31" spans="1:9" ht="80" customHeight="1">
-      <c r="A31" s="129"/>
+      <c r="A31" s="124"/>
       <c r="B31" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="F31" s="107" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="4"/>
       <c r="I31" s="38"/>
     </row>
     <row r="32" spans="1:9" ht="70" customHeight="1">
-      <c r="A32" s="129"/>
+      <c r="A32" s="124"/>
       <c r="B32" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="F32" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="68" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I32" s="38"/>
     </row>
     <row r="33" spans="1:11" ht="75" customHeight="1">
-      <c r="A33" s="129"/>
+      <c r="A33" s="124"/>
       <c r="B33" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" s="35" t="s">
         <v>1</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F33" s="105" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G33" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="H33" s="69" t="s">
-        <v>116</v>
-      </c>
       <c r="I33" s="38"/>
     </row>
     <row r="34" spans="1:11" ht="50" customHeight="1">
-      <c r="A34" s="129"/>
-      <c r="B34" s="112" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="114" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="116" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="118" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="120" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" s="122"/>
-      <c r="H34" s="149"/>
+      <c r="A34" s="124"/>
+      <c r="B34" s="146" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="147" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="148" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="149" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="151"/>
+      <c r="H34" s="127"/>
       <c r="I34" s="38"/>
     </row>
     <row r="35" spans="1:11" ht="50" customHeight="1">
-      <c r="A35" s="129"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="115"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="150"/>
+      <c r="A35" s="124"/>
+      <c r="B35" s="132"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="136"/>
+      <c r="F35" s="130"/>
+      <c r="G35" s="130"/>
+      <c r="H35" s="128"/>
       <c r="I35" s="38"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="141"/>
-      <c r="B36" s="138"/>
-      <c r="C36" s="138"/>
-      <c r="D36" s="138"/>
-      <c r="E36" s="138"/>
-      <c r="F36" s="138"/>
-      <c r="G36" s="138"/>
-      <c r="H36" s="138"/>
+      <c r="A36" s="117"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="118"/>
+      <c r="F36" s="118"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="118"/>
       <c r="I36" s="38"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="142"/>
-      <c r="B37" s="143"/>
-      <c r="C37" s="143"/>
-      <c r="D37" s="143"/>
-      <c r="E37" s="143"/>
-      <c r="F37" s="143"/>
-      <c r="G37" s="143"/>
-      <c r="H37" s="143"/>
+      <c r="A37" s="119"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="120"/>
+      <c r="G37" s="120"/>
+      <c r="H37" s="120"/>
       <c r="I37" s="38"/>
     </row>
     <row r="38" spans="1:11" ht="34">
       <c r="A38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="C38" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="D38" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="E38" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>0</v>
       </c>
       <c r="G38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="I38" s="38"/>
+    </row>
+    <row r="39" spans="1:11" ht="68" customHeight="1">
+      <c r="A39" s="121" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:11" ht="68" customHeight="1">
-      <c r="A39" s="144" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="100" t="s">
+      <c r="D39" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I39" s="38"/>
+    </row>
+    <row r="40" spans="1:11" ht="68" customHeight="1">
+      <c r="A40" s="122"/>
+      <c r="B40" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C40" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="101" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="I39" s="38"/>
-    </row>
-    <row r="40" spans="1:11" ht="68" customHeight="1">
-      <c r="A40" s="145"/>
-      <c r="B40" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E40" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>86</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F40" s="13"/>
       <c r="G40" s="19"/>
       <c r="H40" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I40" s="38"/>
     </row>
     <row r="41" spans="1:11" ht="80" customHeight="1">
-      <c r="A41" s="145"/>
+      <c r="A41" s="122"/>
       <c r="B41" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E41" s="83" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:11" ht="68" customHeight="1">
-      <c r="A42" s="145"/>
+      <c r="A42" s="122"/>
       <c r="B42" s="84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" s="86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E42" s="66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F42" s="87" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G42" s="88"/>
       <c r="H42" s="89"/>
     </row>
     <row r="43" spans="1:11" ht="105" customHeight="1">
-      <c r="A43" s="146"/>
+      <c r="A43" s="123"/>
       <c r="B43" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="56" t="s">
-        <v>76</v>
-      </c>
       <c r="F43" s="57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G43" s="104" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H43" s="102"/>
     </row>
     <row r="44" spans="1:11" ht="43" customHeight="1">
       <c r="A44" s="48"/>
-      <c r="B44" s="140"/>
-      <c r="C44" s="140"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
+      <c r="B44" s="137"/>
+      <c r="C44" s="137"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
       <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:11" ht="63" customHeight="1">
@@ -3358,27 +3341,27 @@
       <c r="H48" s="53"/>
     </row>
     <row r="49" spans="1:8" ht="57" customHeight="1">
-      <c r="A49" s="137"/>
-      <c r="B49" s="137"/>
-      <c r="C49" s="138"/>
-      <c r="D49" s="137"/>
+      <c r="A49" s="138"/>
+      <c r="B49" s="138"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="138"/>
       <c r="E49" s="139"/>
-      <c r="F49" s="135"/>
-      <c r="G49" s="135"/>
-      <c r="H49" s="136"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="141"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="137"/>
-      <c r="B50" s="137"/>
-      <c r="C50" s="138"/>
-      <c r="D50" s="137"/>
+      <c r="A50" s="138"/>
+      <c r="B50" s="138"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="138"/>
       <c r="E50" s="139"/>
-      <c r="F50" s="135"/>
-      <c r="G50" s="135"/>
-      <c r="H50" s="136"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="141"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="137"/>
+      <c r="A51" s="138"/>
       <c r="B51" s="38"/>
       <c r="C51" s="38"/>
       <c r="D51" s="38"/>
@@ -3388,7 +3371,7 @@
       <c r="H51" s="38"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="137"/>
+      <c r="A52" s="138"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
       <c r="D52" s="39"/>
@@ -3398,7 +3381,7 @@
       <c r="H52" s="39"/>
     </row>
     <row r="53" spans="1:8" ht="50" customHeight="1">
-      <c r="A53" s="137"/>
+      <c r="A53" s="138"/>
       <c r="B53" s="41"/>
       <c r="C53" s="41"/>
       <c r="D53" s="41"/>
@@ -3438,27 +3421,27 @@
       <c r="H56" s="53"/>
     </row>
     <row r="57" spans="1:8" ht="43" customHeight="1">
-      <c r="A57" s="137"/>
-      <c r="B57" s="138"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="137"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="118"/>
+      <c r="C57" s="118"/>
+      <c r="D57" s="138"/>
       <c r="E57" s="139"/>
-      <c r="F57" s="135"/>
-      <c r="G57" s="135"/>
-      <c r="H57" s="136"/>
+      <c r="F57" s="140"/>
+      <c r="G57" s="140"/>
+      <c r="H57" s="141"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="137"/>
-      <c r="B58" s="138"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="137"/>
+      <c r="A58" s="138"/>
+      <c r="B58" s="118"/>
+      <c r="C58" s="118"/>
+      <c r="D58" s="138"/>
       <c r="E58" s="139"/>
-      <c r="F58" s="135"/>
-      <c r="G58" s="135"/>
-      <c r="H58" s="136"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="141"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="137"/>
+      <c r="A59" s="138"/>
       <c r="B59" s="38"/>
       <c r="C59" s="38"/>
       <c r="D59" s="38"/>
@@ -3468,7 +3451,7 @@
       <c r="H59" s="38"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="137"/>
+      <c r="A60" s="138"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
       <c r="D60" s="39"/>
@@ -3478,7 +3461,7 @@
       <c r="H60" s="39"/>
     </row>
     <row r="61" spans="1:8" ht="40" customHeight="1">
-      <c r="A61" s="137"/>
+      <c r="A61" s="138"/>
       <c r="B61" s="41"/>
       <c r="C61" s="41"/>
       <c r="D61" s="41"/>
@@ -3518,27 +3501,27 @@
       <c r="H64" s="53"/>
     </row>
     <row r="65" spans="1:8" ht="64" customHeight="1">
-      <c r="A65" s="137"/>
-      <c r="B65" s="137"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="137"/>
+      <c r="A65" s="138"/>
+      <c r="B65" s="138"/>
+      <c r="C65" s="118"/>
+      <c r="D65" s="138"/>
       <c r="E65" s="139"/>
-      <c r="F65" s="135"/>
-      <c r="G65" s="135"/>
-      <c r="H65" s="136"/>
+      <c r="F65" s="140"/>
+      <c r="G65" s="140"/>
+      <c r="H65" s="141"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="137"/>
-      <c r="B66" s="137"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="137"/>
+      <c r="A66" s="138"/>
+      <c r="B66" s="138"/>
+      <c r="C66" s="118"/>
+      <c r="D66" s="138"/>
       <c r="E66" s="139"/>
-      <c r="F66" s="135"/>
-      <c r="G66" s="135"/>
-      <c r="H66" s="136"/>
+      <c r="F66" s="140"/>
+      <c r="G66" s="140"/>
+      <c r="H66" s="141"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="137"/>
+      <c r="A67" s="138"/>
       <c r="B67" s="38"/>
       <c r="C67" s="38"/>
       <c r="D67" s="38"/>
@@ -3548,7 +3531,7 @@
       <c r="H67" s="38"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="137"/>
+      <c r="A68" s="138"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="39"/>
@@ -3558,7 +3541,7 @@
       <c r="H68" s="39"/>
     </row>
     <row r="69" spans="1:8" ht="74" customHeight="1">
-      <c r="A69" s="137"/>
+      <c r="A69" s="138"/>
       <c r="B69" s="41"/>
       <c r="C69" s="41"/>
       <c r="D69" s="41"/>
@@ -3598,27 +3581,27 @@
       <c r="H72" s="53"/>
     </row>
     <row r="73" spans="1:8" ht="83" customHeight="1">
-      <c r="A73" s="137"/>
-      <c r="B73" s="138"/>
-      <c r="C73" s="138"/>
-      <c r="D73" s="137"/>
+      <c r="A73" s="138"/>
+      <c r="B73" s="118"/>
+      <c r="C73" s="118"/>
+      <c r="D73" s="138"/>
       <c r="E73" s="139"/>
-      <c r="F73" s="135"/>
-      <c r="G73" s="135"/>
-      <c r="H73" s="136"/>
+      <c r="F73" s="140"/>
+      <c r="G73" s="140"/>
+      <c r="H73" s="141"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="137"/>
-      <c r="B74" s="138"/>
-      <c r="C74" s="138"/>
-      <c r="D74" s="137"/>
+      <c r="A74" s="138"/>
+      <c r="B74" s="118"/>
+      <c r="C74" s="118"/>
+      <c r="D74" s="138"/>
       <c r="E74" s="139"/>
-      <c r="F74" s="135"/>
-      <c r="G74" s="135"/>
-      <c r="H74" s="136"/>
+      <c r="F74" s="140"/>
+      <c r="G74" s="140"/>
+      <c r="H74" s="141"/>
     </row>
     <row r="75" spans="1:8" ht="16" customHeight="1">
-      <c r="A75" s="137"/>
+      <c r="A75" s="138"/>
       <c r="B75" s="38"/>
       <c r="C75" s="38"/>
       <c r="D75" s="38"/>
@@ -3628,7 +3611,7 @@
       <c r="H75" s="38"/>
     </row>
     <row r="76" spans="1:8" ht="36" customHeight="1">
-      <c r="A76" s="137"/>
+      <c r="A76" s="138"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
       <c r="D76" s="39"/>
@@ -3638,7 +3621,7 @@
       <c r="H76" s="39"/>
     </row>
     <row r="77" spans="1:8" ht="86" customHeight="1">
-      <c r="A77" s="137"/>
+      <c r="A77" s="138"/>
       <c r="B77" s="41"/>
       <c r="C77" s="41"/>
       <c r="D77" s="41"/>
@@ -3678,27 +3661,27 @@
       <c r="H80" s="53"/>
     </row>
     <row r="81" spans="1:8" ht="29" customHeight="1">
-      <c r="A81" s="137"/>
-      <c r="B81" s="137"/>
-      <c r="C81" s="138"/>
-      <c r="D81" s="137"/>
+      <c r="A81" s="138"/>
+      <c r="B81" s="138"/>
+      <c r="C81" s="118"/>
+      <c r="D81" s="138"/>
       <c r="E81" s="139"/>
-      <c r="F81" s="135"/>
-      <c r="G81" s="135"/>
-      <c r="H81" s="136"/>
+      <c r="F81" s="140"/>
+      <c r="G81" s="140"/>
+      <c r="H81" s="141"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="137"/>
-      <c r="B82" s="137"/>
-      <c r="C82" s="138"/>
-      <c r="D82" s="137"/>
+      <c r="A82" s="138"/>
+      <c r="B82" s="138"/>
+      <c r="C82" s="118"/>
+      <c r="D82" s="138"/>
       <c r="E82" s="139"/>
-      <c r="F82" s="135"/>
-      <c r="G82" s="135"/>
-      <c r="H82" s="136"/>
+      <c r="F82" s="140"/>
+      <c r="G82" s="140"/>
+      <c r="H82" s="141"/>
     </row>
     <row r="83" spans="1:8" ht="35" customHeight="1">
-      <c r="A83" s="137"/>
+      <c r="A83" s="138"/>
       <c r="B83" s="38"/>
       <c r="C83" s="38"/>
       <c r="D83" s="38"/>
@@ -3708,7 +3691,7 @@
       <c r="H83" s="38"/>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="137"/>
+      <c r="A84" s="138"/>
       <c r="B84" s="38"/>
       <c r="C84" s="38"/>
       <c r="D84" s="38"/>
@@ -3718,7 +3701,7 @@
       <c r="H84" s="38"/>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="137"/>
+      <c r="A85" s="138"/>
       <c r="B85" s="38"/>
       <c r="C85" s="38"/>
       <c r="D85" s="38"/>
@@ -3732,23 +3715,47 @@
     <row r="113" ht="25" customHeight="1"/>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A36:H37"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:H19"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A27:H28"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
     <mergeCell ref="B44:H44"/>
     <mergeCell ref="A81:A85"/>
     <mergeCell ref="B81:B82"/>
@@ -3765,47 +3772,23 @@
     <mergeCell ref="E73:E74"/>
     <mergeCell ref="F73:F74"/>
     <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A36:H37"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:H19"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A27:H28"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>